<commit_message>
add barnes et al. 2019 data to overview plot
</commit_message>
<xml_diff>
--- a/data/literature.xlsx
+++ b/data/literature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sk/GDrive/science/manuscripts/2020_nitrate_reductase_enzyme_effects/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sk/My Drive/science/manuscripts/2020_nitrate_reductase_enzyme_effects/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D9F5C7-EA77-314A-B404-B07734075CC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6311804F-BC22-D544-BE3D-5AA9EE8B0E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26540" yWindow="16480" windowWidth="26020" windowHeight="16980" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12720" yWindow="2420" windowWidth="33680" windowHeight="22740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="terrestrial_data" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7837" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8035" uniqueCount="89">
   <si>
     <t>PC</t>
   </si>
@@ -273,15 +273,45 @@
   <si>
     <t>AA</t>
   </si>
+  <si>
+    <t>Barnes et al., 2019</t>
+  </si>
+  <si>
+    <t>DK-3m</t>
+  </si>
+  <si>
+    <t>EB-2.5m</t>
+  </si>
+  <si>
+    <t>EK-3m</t>
+  </si>
+  <si>
+    <t>FR-2.2m</t>
+  </si>
+  <si>
+    <t>FB-2.5m</t>
+  </si>
+  <si>
+    <t>FK-3m</t>
+  </si>
+  <si>
+    <t>GR-2.2m</t>
+  </si>
+  <si>
+    <t>GB-2.5m</t>
+  </si>
+  <si>
+    <t>HR-2.2m</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -293,6 +323,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -318,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -328,8 +364,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,30 +649,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58311B85-0A1E-B941-93FF-E3E0B3C8FBFD}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -641,16 +680,16 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="12">
         <v>22.57</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="12">
         <v>14.89</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -658,17 +697,17 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
+      <c r="A3" s="1" t="str">
         <f>A$2</f>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="12">
         <v>20.82</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="12">
         <v>13.31</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -676,17 +715,17 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
+      <c r="A4" s="1" t="str">
         <f t="shared" ref="A4:A11" si="0">A$2</f>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="12">
         <v>50.58</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="12">
         <v>22.53</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -694,17 +733,17 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
+      <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="12">
         <v>8.9600000000000009</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="12">
         <v>9.9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -712,17 +751,17 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
+      <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="12">
         <v>26.62</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="12">
         <v>17.600000000000001</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -730,17 +769,17 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
+      <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="12">
         <v>71.86</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="12">
         <v>37.93</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -748,17 +787,17 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="str">
+      <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="12">
         <v>78.319999999999993</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="12">
         <v>43.76</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -766,17 +805,17 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="str">
+      <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="12">
         <v>9.69</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="12">
         <v>6.01</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -784,17 +823,17 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="str">
+      <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="12">
         <v>19.09</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="12">
         <v>13.78</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -802,17 +841,17 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="str">
+      <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Böttcher et al., 1990</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="12">
         <v>37.090000000000003</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="12">
         <v>25.67</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -820,434 +859,462 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="12">
         <v>9.8820058997050104</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="12">
         <v>1.5173034031225201</v>
       </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
+      <c r="A13" s="1" t="str">
         <f>A$12</f>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="12">
         <v>8.9478859390363805</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="12">
         <v>2.6654675396311398</v>
       </c>
+      <c r="D13" s="12"/>
       <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="str">
+      <c r="A14" s="1" t="str">
         <f t="shared" ref="A14:A30" si="1">A$12</f>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="12">
         <v>11.0127826941986</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="12">
         <v>3.1004628630357001</v>
       </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="str">
+      <c r="A15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="12">
         <v>10.3736479842674</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="12">
         <v>3.90658800393313</v>
       </c>
+      <c r="D15" s="12"/>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="str">
+      <c r="A16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="12">
         <v>13.3726647000983</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="12">
         <v>4.2909801664388301</v>
       </c>
+      <c r="D16" s="12"/>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="str">
+      <c r="A17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="12">
         <v>14.5034414945919</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="12">
         <v>3.4838957239129802</v>
       </c>
+      <c r="D17" s="12"/>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="str">
+      <c r="A18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="12">
         <v>13.8643067846607</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="12">
         <v>2.4119720843226098</v>
       </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="str">
+      <c r="A19" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="12">
         <v>17.4041297935103</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="12">
         <v>4.3562846247931502</v>
       </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="str">
+      <c r="A20" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="12">
         <v>18.879056047197601</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="12">
         <v>6.7680408662493701</v>
       </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="str">
+      <c r="A21" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="12">
         <v>19.616519174041301</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="12">
         <v>7.3763580113677198</v>
       </c>
+      <c r="D21" s="12"/>
       <c r="E21" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="str">
+      <c r="A22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="12">
         <v>21.337266470009801</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="12">
         <v>6.6900736263999798</v>
       </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="str">
+      <c r="A23" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="12">
         <v>22.271386430678401</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="12">
         <v>8.2004460752572097</v>
       </c>
+      <c r="D23" s="12"/>
       <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
+      <c r="A24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="12">
         <v>23.992133726647001</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="12">
         <v>8.8800153488260491</v>
       </c>
+      <c r="D24" s="12"/>
       <c r="E24" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="str">
+      <c r="A25" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="12">
         <v>25.172074729596801</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="12">
         <v>9.3655179029666407</v>
       </c>
+      <c r="D25" s="12"/>
       <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="str">
+      <c r="A26" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="12">
         <v>30.727630285152401</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="12">
         <v>12.6717509652972</v>
       </c>
+      <c r="D26" s="12"/>
       <c r="E26" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="str">
+      <c r="A27" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="12">
         <v>32.300884955752203</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="12">
         <v>12.7174616878912</v>
       </c>
+      <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="str">
+      <c r="A28" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="12">
         <v>36.9223205506391</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="12">
         <v>13.098688155023099</v>
       </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="str">
+      <c r="A29" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="12">
         <v>39.085545722713803</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="12">
         <v>15.826174544931201</v>
       </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="str">
+      <c r="A30" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Aravena and Robertson, 1998</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="12">
         <v>38.8888888888888</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="12">
         <v>16.4119241192411</v>
       </c>
+      <c r="D30" s="12"/>
       <c r="E30" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="12">
         <v>4.8165226324078603</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="12">
         <v>-5.3671713280545298E-2</v>
       </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="str">
-        <f>A$31</f>
+      <c r="A32" s="1" t="str">
+        <f t="shared" ref="A32:A39" si="2">A$31</f>
         <v>Cey et al., 1999</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="12">
         <v>6.5343361583231996</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="12">
         <v>0.77297044744993004</v>
       </c>
+      <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="str">
-        <f>A$31</f>
+      <c r="A33" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>Cey et al., 1999</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="12">
         <v>7.4077855854350503</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="12">
         <v>0.113810270833914</v>
       </c>
+      <c r="D33" s="12"/>
       <c r="E33" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="str">
-        <f>A$31</f>
+      <c r="A34" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>Cey et al., 1999</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="12">
         <v>8.3201056973207397</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="12">
         <v>1.8965552451057699</v>
       </c>
+      <c r="D34" s="12"/>
       <c r="E34" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="str">
-        <f>A$31</f>
+      <c r="A35" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>Cey et al., 1999</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="12">
         <v>8.3437375265712994</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="12">
         <v>1.6537732025112399</v>
       </c>
+      <c r="D35" s="12"/>
       <c r="E35" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="str">
-        <f>A$31</f>
+      <c r="A36" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>Cey et al., 1999</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="12">
         <v>8.6424809785047003</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="12">
         <v>1.4520571681410399</v>
       </c>
+      <c r="D36" s="12"/>
       <c r="E36" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="str">
-        <f>A$31</f>
+      <c r="A37" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>Cey et al., 1999</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="12">
         <v>13.9347730570846</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="12">
         <v>3.5005801594742301</v>
       </c>
+      <c r="D37" s="12"/>
       <c r="E37" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="str">
-        <f>A$31</f>
+      <c r="A38" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>Cey et al., 1999</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="12">
         <v>17.018165953457199</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="12">
         <v>8.0131379046805709</v>
       </c>
+      <c r="D38" s="12"/>
       <c r="E38" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="str">
-        <f>A$31</f>
+      <c r="A39" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>Cey et al., 1999</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="12">
         <v>25.2193776358578</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="12">
         <v>11.4305030833542</v>
       </c>
+      <c r="D39" s="12"/>
       <c r="E39" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="12">
         <v>4.7</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="12">
         <v>0.3</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -1255,17 +1322,17 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="str">
-        <f>A$40</f>
+      <c r="A41" s="1" t="str">
+        <f t="shared" ref="A41:A57" si="3">A$40</f>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="12">
         <v>15.9</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="12">
         <v>8.5</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -1273,17 +1340,17 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="str">
-        <f>A$40</f>
+      <c r="A42" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="12">
         <v>20.5</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="12">
         <v>12.5</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="12" t="s">
         <v>15</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -1291,17 +1358,17 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="str">
-        <f>A$40</f>
+      <c r="A43" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="12">
         <v>29.2</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="12">
         <v>17.8</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -1309,17 +1376,17 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="str">
-        <f>A$40</f>
+      <c r="A44" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="12">
         <v>48.8</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="12">
         <v>17</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -1327,17 +1394,17 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="str">
-        <f>A$40</f>
+      <c r="A45" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="12">
         <v>14.5</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="12">
         <v>8.9</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -1345,17 +1412,17 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="str">
-        <f>A$40</f>
+      <c r="A46" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="12">
         <v>14.6</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="12">
         <v>8.1</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="12" t="s">
         <v>19</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -1363,17 +1430,17 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="str">
-        <f>A$40</f>
+      <c r="A47" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="12">
         <v>7.7</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="12">
         <v>3.3</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -1381,17 +1448,17 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="str">
-        <f>A$40</f>
+      <c r="A48" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="12">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -1399,17 +1466,17 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="str">
-        <f>A$40</f>
+      <c r="A49" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="12">
         <v>20.8</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="12">
         <v>10.3</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -1417,17 +1484,17 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="str">
-        <f>A$40</f>
+      <c r="A50" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="12">
         <v>7.5</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="12">
         <v>3.5</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="12" t="s">
         <v>23</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -1435,17 +1502,17 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="str">
-        <f>A$40</f>
+      <c r="A51" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="12">
         <v>7.4</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -1453,17 +1520,17 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="str">
-        <f>A$40</f>
+      <c r="A52" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="12">
         <v>16.8</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="12">
         <v>7.5</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -1471,17 +1538,17 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="str">
-        <f>A$40</f>
+      <c r="A53" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="12">
         <v>6</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="12">
         <v>1.7</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -1489,17 +1556,17 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="str">
-        <f>A$40</f>
+      <c r="A54" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="12">
         <v>4.5999999999999996</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="12">
         <v>0.4</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -1507,17 +1574,17 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="str">
-        <f>A$40</f>
+      <c r="A55" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="12">
         <v>10.1</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="12">
         <v>6.2</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -1525,17 +1592,17 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="str">
-        <f>A$40</f>
+      <c r="A56" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="12">
         <v>3.8</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="12">
         <v>0.5</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -1543,17 +1610,17 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="str">
-        <f>A$40</f>
+      <c r="A57" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Mengis et al., 1999</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="12">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="12">
         <v>1</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="12" t="s">
         <v>30</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -1561,599 +1628,1763 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="12">
+        <v>15.604616605104844</v>
+      </c>
+      <c r="C58" s="12">
+        <v>10.149657881305242</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="12">
+        <v>17.11123803214614</v>
+      </c>
+      <c r="C59" s="12">
+        <v>10.347333914712738</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="12">
+        <v>17.542945991129727</v>
+      </c>
+      <c r="C60" s="12">
+        <v>10.259917894026843</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" s="12">
+        <v>17.168642697957441</v>
+      </c>
+      <c r="C61" s="12">
+        <v>10.450513085242125</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="12">
+        <v>18.579836172755357</v>
+      </c>
+      <c r="C62" s="12">
+        <v>10.735342827426255</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" s="12">
+        <v>18.310650136818143</v>
+      </c>
+      <c r="C63" s="12">
+        <v>10.597579698730062</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" s="12">
+        <v>16.942195094051478</v>
+      </c>
+      <c r="C64" s="12">
+        <v>10.134818603215184</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="12">
+        <v>15.368509294931712</v>
+      </c>
+      <c r="C65" s="12">
+        <v>9.7133995786493408</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="12">
+        <v>16.352363025950794</v>
+      </c>
+      <c r="C66" s="12">
+        <v>9.6659431301204499</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" s="13">
+        <v>15.622965112456939</v>
+      </c>
+      <c r="C67" s="13">
+        <v>8.779208587944261</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="13">
+        <v>16.785165862365126</v>
+      </c>
+      <c r="C68" s="13">
+        <v>8.5487706121999505</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B69" s="12">
+        <v>17.334822938442599</v>
+      </c>
+      <c r="C69" s="12">
+        <v>8.5446068441977481</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="12">
+        <v>17.482635476892607</v>
+      </c>
+      <c r="C70" s="12">
+        <v>8.604868133156458</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" s="12">
+        <v>17.622485996404809</v>
+      </c>
+      <c r="C71" s="12">
+        <v>8.6207237656903875</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="12">
+        <v>17.415377401198036</v>
+      </c>
+      <c r="C72" s="12">
+        <v>8.5062392977153785</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="12">
+        <v>17.214963650498319</v>
+      </c>
+      <c r="C73" s="12">
+        <v>8.4637528838566212</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="12">
+        <v>17.228919544203311</v>
+      </c>
+      <c r="C74" s="12">
+        <v>8.4237752414597651</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="13">
+        <v>28.146855775132824</v>
+      </c>
+      <c r="C75" s="13">
+        <v>14.737825459244309</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="13">
+        <v>26.924563453256976</v>
+      </c>
+      <c r="C76" s="13">
+        <v>13.545291406620823</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="12">
+        <v>26.362317235427035</v>
+      </c>
+      <c r="C77" s="12">
+        <v>12.871461820044605</v>
+      </c>
+      <c r="D77" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="12">
+        <v>25.484353630468739</v>
+      </c>
+      <c r="C78" s="12">
+        <v>12.210023024019296</v>
+      </c>
+      <c r="D78" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="12">
+        <v>24.826571953797171</v>
+      </c>
+      <c r="C79" s="12">
+        <v>11.74042452482562</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="12">
+        <v>24.065620716562805</v>
+      </c>
+      <c r="C80" s="12">
+        <v>11.433056752739486</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="12">
+        <v>23.757605428198996</v>
+      </c>
+      <c r="C81" s="12">
+        <v>11.293151901473223</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="12">
+        <v>23.281814888216154</v>
+      </c>
+      <c r="C82" s="12">
+        <v>10.506277580666382</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83" s="12">
+        <v>23.32048162643002</v>
+      </c>
+      <c r="C83" s="12">
+        <v>11.096873686681153</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="12">
+        <v>17.49716894752779</v>
+      </c>
+      <c r="C84" s="12">
+        <v>10.577475112609827</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" s="12">
+        <v>17.333537828823683</v>
+      </c>
+      <c r="C85" s="12">
+        <v>10.969871458394735</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" s="12">
+        <v>17.876294463440093</v>
+      </c>
+      <c r="C86" s="12">
+        <v>11.260449972632374</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" s="12">
+        <v>18.821637357363098</v>
+      </c>
+      <c r="C87" s="12">
+        <v>11.590579576203336</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88" s="12">
+        <v>18.690807022198406</v>
+      </c>
+      <c r="C88" s="12">
+        <v>11.256332924636858</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" s="12">
+        <v>19.218558866399327</v>
+      </c>
+      <c r="C89" s="12">
+        <v>11.823536539475271</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" s="12">
+        <v>19.16887306867919</v>
+      </c>
+      <c r="C90" s="12">
+        <v>11.400726240662149</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" s="12">
+        <v>18.925753862899654</v>
+      </c>
+      <c r="C91" s="12">
+        <v>10.044291082078654</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="12">
+        <v>18.104570755581769</v>
+      </c>
+      <c r="C92" s="12">
+        <v>9.4698841712748951</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="12">
+        <v>16.697835467141463</v>
+      </c>
+      <c r="C93" s="12">
+        <v>8.4433685505222389</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="12">
+        <v>18.463832326633515</v>
+      </c>
+      <c r="C94" s="12">
+        <v>10.371928305638047</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="12">
+        <v>14.247655846283042</v>
+      </c>
+      <c r="C95" s="12">
+        <v>8.9401638073561607</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" s="12">
+        <v>15.062552143174436</v>
+      </c>
+      <c r="C96" s="12">
+        <v>8.7936123979708594</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" s="12">
+        <v>15.031373685396275</v>
+      </c>
+      <c r="C97" s="12">
+        <v>9.3840974080494526</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" s="12">
+        <v>15.390548731310528</v>
+      </c>
+      <c r="C98" s="12">
+        <v>9.8098901674089518</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" s="12">
+        <v>15.499173435668549</v>
+      </c>
+      <c r="C99" s="12">
+        <v>10.035127632790109</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B100" s="12">
+        <v>15.956771293185691</v>
+      </c>
+      <c r="C100" s="12">
+        <v>9.8524199302965521</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101" s="12">
+        <v>15.520265211729633</v>
+      </c>
+      <c r="C101" s="12">
+        <v>10.004726921767553</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B102" s="12">
+        <v>15.272822765694535</v>
+      </c>
+      <c r="C102" s="12">
+        <v>9.345829392508163</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B103" s="12">
+        <v>15.296085202653552</v>
+      </c>
+      <c r="C103" s="12">
+        <v>9.4165222421964465</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B104" s="12">
+        <v>13.356848470259422</v>
+      </c>
+      <c r="C104" s="12">
+        <v>6.8315532441229863</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B105" s="12">
+        <v>12.716456504845667</v>
+      </c>
+      <c r="C105" s="12">
+        <v>6.224868712861368</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B106" s="12">
+        <v>14.063476931787399</v>
+      </c>
+      <c r="C106" s="12">
+        <v>6.7931756495317401</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B107" s="12">
+        <v>12.967054469279532</v>
+      </c>
+      <c r="C107" s="12">
+        <v>6.7062171664194441</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108" s="12">
+        <v>12.971336814385666</v>
+      </c>
+      <c r="C108" s="12">
+        <v>6.690366076097666</v>
+      </c>
+      <c r="D108" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109" s="12">
+        <v>12.934569016821563</v>
+      </c>
+      <c r="C109" s="12">
+        <v>6.3151404176370463</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" s="12">
+        <v>21.576972720164516</v>
+      </c>
+      <c r="C110" s="12">
+        <v>13.311111507320817</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B111" s="12">
+        <v>15.531820619820197</v>
+      </c>
+      <c r="C111" s="12">
+        <v>8.0501931543480278</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112" s="12">
+        <v>14.299115127934137</v>
+      </c>
+      <c r="C112" s="12">
+        <v>7.1035802074443026</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B113" s="12">
+        <v>13.921033401334849</v>
+      </c>
+      <c r="C113" s="12">
+        <v>7.0327932683007841</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B114" s="12">
+        <v>13.821714939443385</v>
+      </c>
+      <c r="C114" s="12">
+        <v>7.2799995941702376</v>
+      </c>
+      <c r="D114" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B115" s="12">
+        <v>20.570151304814775</v>
+      </c>
+      <c r="C115" s="12">
+        <v>12.252148124986833</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B116" s="12">
+        <v>23.837261374610136</v>
+      </c>
+      <c r="C116" s="12">
+        <v>13.692269115188298</v>
+      </c>
+      <c r="D116" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B117" s="12">
+        <v>23.544100889931869</v>
+      </c>
+      <c r="C117" s="12">
+        <v>13.429799663315951</v>
+      </c>
+      <c r="D117" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B118" s="12">
+        <v>23.372823300166491</v>
+      </c>
+      <c r="C118" s="12">
+        <v>13.222304536683803</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B119" s="12">
+        <v>23.245057449677706</v>
+      </c>
+      <c r="C119" s="12">
+        <v>13.274384258729841</v>
+      </c>
+      <c r="D119" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B120" s="12">
+        <v>23.170780037292538</v>
+      </c>
+      <c r="C120" s="12">
+        <v>13.073433564631038</v>
+      </c>
+      <c r="D120" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B121" s="12">
+        <v>22.956673174077878</v>
+      </c>
+      <c r="C121" s="12">
+        <v>13.354687379792159</v>
+      </c>
+      <c r="D121" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B122" s="12">
+        <v>22.858051034170408</v>
+      </c>
+      <c r="C122" s="12">
+        <v>13.432358256240896</v>
+      </c>
+      <c r="D122" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B123" s="12">
+        <v>22.760331707638958</v>
+      </c>
+      <c r="C123" s="12">
+        <v>12.943203290176399</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B124" s="12">
         <v>7.2222222222222197</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C124" s="12">
         <v>4.5157981803142997</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="D124" s="12"/>
+      <c r="E124" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="str">
-        <f>A$58</f>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="str">
+        <f>A$124</f>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B125" s="12">
         <v>8.8580246913580201</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C125" s="12">
         <v>5.4250528444076798</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="D125" s="12"/>
+      <c r="E125" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="str">
-        <f t="shared" ref="A60:A67" si="2">A$58</f>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="str">
+        <f t="shared" ref="A126:A133" si="4">A$124</f>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B126" s="12">
         <v>9.5679012345679002</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C126" s="12">
         <v>4.5300615752228603</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="D126" s="12"/>
+      <c r="E126" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="str">
-        <f t="shared" si="2"/>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B127" s="12">
         <v>12.0679012345679</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C127" s="12">
         <v>7.8987960665379999</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="D127" s="12"/>
+      <c r="E127" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="str">
-        <f t="shared" si="2"/>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B128" s="12">
         <v>15</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C128" s="12">
         <v>8.0903225806451609</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="D128" s="12"/>
+      <c r="E128" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="str">
-        <f t="shared" si="2"/>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B129" s="12">
         <v>19.351851851851801</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C129" s="12">
         <v>9.78715191618417</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="D129" s="12"/>
+      <c r="E129" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="str">
-        <f t="shared" si="2"/>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B130" s="12">
         <v>19.382716049382701</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C130" s="12">
         <v>12.1692123885672</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="D130" s="12"/>
+      <c r="E130" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="str">
-        <f t="shared" si="2"/>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B131" s="12">
         <v>23.518518518518501</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C131" s="12">
         <v>12.8541494347945</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="D131" s="12"/>
+      <c r="E131" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="str">
-        <f t="shared" si="2"/>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B132" s="12">
         <v>24.7222222222222</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C132" s="12">
         <v>14.6180314309346</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="D132" s="12"/>
+      <c r="E132" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="str">
-        <f t="shared" si="2"/>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Lehmann et al., 2003</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B133" s="12">
         <v>26.9444444444444</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C133" s="12">
         <v>15.664846980976</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="D133" s="12"/>
+      <c r="E133" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B134" s="12">
         <v>5.9763146760000003</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C134" s="12">
         <v>4.1355326999999997E-2</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="D134" s="12"/>
+      <c r="E134" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B135" s="12">
         <v>7.1925372430000003</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C135" s="12">
         <v>1.013675455</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="D135" s="12"/>
+      <c r="E135" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B136" s="12">
         <v>6.7019126839999998</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C136" s="12">
         <v>0.44175008199999999</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="D136" s="12"/>
+      <c r="E136" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B137" s="12">
         <v>6.5369613229999999</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C137" s="12">
         <v>0.92720522599999999</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="D137" s="12"/>
+      <c r="E137" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B138" s="12">
         <v>7.0186568920000001</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C138" s="12">
         <v>0.59589266399999996</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="D138" s="12"/>
+      <c r="E138" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B139" s="12">
         <v>7.3391606749999996</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C139" s="12">
         <v>1.241599699</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="D139" s="12"/>
+      <c r="E139" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B140" s="12">
         <v>7.7461346869999996</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C140" s="12">
         <v>1.892006203</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="D140" s="12"/>
+      <c r="E140" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B141" s="12">
         <v>7.5793035389999996</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C141" s="12">
         <v>1.4004417499999999</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="D141" s="12"/>
+      <c r="E141" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B142" s="12">
         <v>7.9815780820000004</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C142" s="12">
         <v>1.396212228</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="D142" s="12"/>
+      <c r="E142" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B143" s="12">
         <v>8.0609991070000007</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C143" s="12">
         <v>1.6382348790000001</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="D143" s="12"/>
+      <c r="E143" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B144" s="12">
         <v>8.4581042340000003</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C144" s="12">
         <v>2.3605432589999999</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="D144" s="12"/>
+      <c r="E144" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B145" s="12">
         <v>8.4595140749999995</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C145" s="12">
         <v>2.1993514730000001</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="D145" s="12"/>
+      <c r="E145" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B146" s="12">
         <v>9.1028713759999995</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C146" s="12">
         <v>2.3549038960000002</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="D146" s="12"/>
+      <c r="E146" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B147" s="12">
         <v>9.6682174910000001</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C147" s="12">
         <v>2.432445134</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="D147" s="12"/>
+      <c r="E147" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B148" s="12">
         <v>9.4233751590000008</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C148" s="12">
         <v>1.943700362</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="D148" s="12"/>
+      <c r="E148" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B149" s="12">
         <v>10.06532262</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C149" s="12">
         <v>2.5851778749999998</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="D149" s="12"/>
+      <c r="E149" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B150" s="12">
         <v>10.066732460000001</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C150" s="12">
         <v>2.6683584749999998</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="D150" s="12"/>
+      <c r="E150" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B151" s="12">
         <v>10.62690916</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C151" s="12">
         <v>3.3911368020000001</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="D151" s="12"/>
+      <c r="E151" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B152" s="12">
         <v>11.84313173</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C152" s="12">
         <v>3.8756520509999999</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="D152" s="12"/>
+      <c r="E152" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B153" s="12">
         <v>11.18661591</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C153" s="12">
         <v>2.8934630389999998</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="D153" s="12"/>
+      <c r="E153" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B154" s="12">
         <v>12.0813948</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C154" s="12">
         <v>3.625640303</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="D154" s="12"/>
+      <c r="E154" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B155" s="12">
         <v>12.40236853</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C155" s="12">
         <v>3.4592791009999999</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="D155" s="12"/>
+      <c r="E155" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B156" s="12">
         <v>11.906574559999999</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C156" s="12">
         <v>3.6138916299999999</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="D156" s="12"/>
+      <c r="E156" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B157" s="12">
         <v>12.713003430000001</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C157" s="12">
         <v>4.0951172519999997</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="D157" s="12"/>
+      <c r="E157" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B158" s="12">
         <v>13.11715776</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C158" s="12">
         <v>4.2548991960000002</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="D158" s="12"/>
+      <c r="E158" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B159" s="12">
         <v>13.35213121</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C159" s="12">
         <v>6.9293669820000003</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="D159" s="12"/>
+      <c r="E159" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B160" s="12">
         <v>13.8380563</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C160" s="12">
         <v>4.8949668690000001</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="D160" s="12"/>
+      <c r="E160" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B161" s="12">
         <v>15.701395740000001</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C161" s="12">
         <v>6.0265989940000004</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="D161" s="12"/>
+      <c r="E161" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B162" s="12">
         <v>15.04206025</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C162" s="12">
         <v>5.7737675639999999</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="D162" s="12"/>
+      <c r="E162" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B163" s="12">
         <v>22.54476244</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C163" s="12">
         <v>12.707364070000001</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="D163" s="12"/>
+      <c r="E163" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B164" s="12">
         <v>22.530664030000001</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C164" s="12">
         <v>13.018468909999999</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="D164" s="12"/>
+      <c r="E164" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B165" s="12">
         <v>26.367780440000001</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C165" s="12">
         <v>16.449081249999999</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="D165" s="12"/>
+      <c r="E165" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -85914,7 +87145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE2EA39-70B9-D94C-8E5A-7F7785F781D6}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -85984,7 +87215,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" ref="A3:A10" si="0">$A$2</f>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -86011,7 +87242,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="0"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -86038,7 +87269,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="0"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -86065,7 +87296,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="0"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -86092,7 +87323,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="0"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -86119,7 +87350,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="0"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -86146,7 +87377,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="0"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -86173,7 +87404,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="0"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -86200,7 +87431,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="str">
-        <f t="shared" ref="A11:A16" si="0">$A$2</f>
+        <f t="shared" ref="A11:A16" si="1">$A$2</f>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -86227,7 +87458,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -86254,7 +87485,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -86281,7 +87512,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -86308,7 +87539,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -86335,7 +87566,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -86362,7 +87593,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" ref="A17:A22" si="2">$A$2</f>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -86389,7 +87620,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="2"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -86416,7 +87647,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="2"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -86443,7 +87674,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="2"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -86470,7 +87701,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="2"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -86497,7 +87728,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="str">
-        <f>$A$2</f>
+        <f t="shared" si="2"/>
         <v>Granger et al., 2008</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -86571,7 +87802,7 @@
         <v>1.5</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" ref="G24:G27" si="1">E24/C24</f>
+        <f t="shared" ref="G24:G27" si="3">E24/C24</f>
         <v>0.93063583815028905</v>
       </c>
       <c r="H24" s="2">
@@ -86600,11 +87831,11 @@
         <v>0.8</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.90045248868778272</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" ref="H24:H45" si="2">SQRT((D25/C25)^2 + (F25/E25)^2)*G25</f>
+        <f t="shared" ref="H25:H45" si="4">SQRT((D25/C25)^2 + (F25/E25)^2)*G25</f>
         <v>4.8711860478261405E-2</v>
       </c>
     </row>
@@ -86629,11 +87860,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.84126984126984139</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.2071526398652409E-2</v>
       </c>
     </row>
@@ -86658,11 +87889,11 @@
         <v>0.6</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.91160220994475127</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.4855846017663119E-2</v>
       </c>
     </row>
@@ -86689,7 +87920,7 @@
         <v>0.54</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1100565194697799E-2</v>
       </c>
     </row>
@@ -86717,13 +87948,13 @@
         <v>0.5</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.4641879288884769E-2</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="str">
-        <f t="shared" ref="A30:A45" si="3">A$28</f>
+        <f t="shared" ref="A30:A45" si="5">A$28</f>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -86745,13 +87976,13 @@
         <v>0.53</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6100775830944155E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -86773,13 +88004,13 @@
         <v>0.52</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.7609887562592094E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -86801,13 +88032,13 @@
         <v>0.47</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.8532518691454558E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -86829,13 +88060,13 @@
         <v>0.62</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.4869870736291245E-2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -86857,13 +88088,13 @@
         <v>0.68</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.0042520349908901E-2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -86885,13 +88116,13 @@
         <v>0.6</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.9322365462485052E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -86913,13 +88144,13 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.3475810522830428E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -86941,13 +88172,13 @@
         <v>0.46</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.9859610697852394E-2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -86969,13 +88200,13 @@
         <v>0.48</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.8785006117096578E-2</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -86997,13 +88228,13 @@
         <v>0.51</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.10710291885640981</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -87025,13 +88256,13 @@
         <v>0.43</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.4187254653115407E-2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -87053,13 +88284,13 @@
         <v>0.48</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.1334534456899027E-2</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -87081,13 +88312,13 @@
         <v>0.48</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.2300540852736059E-2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -87109,13 +88340,13 @@
         <v>0.5</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.4686248831990148E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -87137,13 +88368,13 @@
         <v>0.46</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.4305017068368901E-2</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Frey et al., 2014</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -87165,7 +88396,7 @@
         <v>0.53</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.8124174735881013E-2</v>
       </c>
     </row>

</xml_diff>